<commit_message>
Finish the LC Margin Calculator
</commit_message>
<xml_diff>
--- a/lc_margin/main/tests/files/LCmargin_train.xlsx
+++ b/lc_margin/main/tests/files/LCmargin_train.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="270" windowWidth="15780" windowHeight="9030" activeTab="3"/>
+    <workbookView xWindow="3150" yWindow="270" windowWidth="15780" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="原始輸入表格" sheetId="2" r:id="rId1"/>
-    <sheet name="upload" sheetId="4" r:id="rId2"/>
-    <sheet name="轉換後表格_T2" sheetId="1" r:id="rId3"/>
-    <sheet name="轉換後表格_T1" sheetId="3" r:id="rId4"/>
+    <sheet name="upload" sheetId="4" r:id="rId1"/>
+    <sheet name="upload_T1" sheetId="5" r:id="rId2"/>
+    <sheet name="原始輸入表格" sheetId="2" r:id="rId3"/>
+    <sheet name="轉換後表格_T2" sheetId="1" r:id="rId4"/>
+    <sheet name="轉換後表格_T1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="117">
   <si>
     <t>Dimension</t>
   </si>
@@ -1372,524 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BV6" sqref="BV6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>94</v>
-      </c>
-      <c r="T1" t="s">
-        <v>95</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BA1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2">
-        <v>5.7</v>
-      </c>
-      <c r="C2">
-        <v>86.25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>144</v>
-      </c>
-      <c r="G2">
-        <v>10.6</v>
-      </c>
-      <c r="H2">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="I2">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>0.10709399999999999</v>
-      </c>
-      <c r="K2">
-        <v>409.23145099999999</v>
-      </c>
-      <c r="L2">
-        <v>0.49662899999999999</v>
-      </c>
-      <c r="M2">
-        <v>8.5</v>
-      </c>
-      <c r="N2">
-        <v>8.5</v>
-      </c>
-      <c r="O2">
-        <v>18.5</v>
-      </c>
-      <c r="P2">
-        <v>18.5</v>
-      </c>
-      <c r="Q2">
-        <v>403</v>
-      </c>
-      <c r="R2">
-        <v>2.1347749999999999</v>
-      </c>
-      <c r="S2">
-        <v>276.91503</v>
-      </c>
-      <c r="T2">
-        <v>10.417676999999999</v>
-      </c>
-      <c r="U2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2">
-        <v>24.8</v>
-      </c>
-      <c r="W2">
-        <v>68.8</v>
-      </c>
-      <c r="X2">
-        <v>3.0096000000000001E-2</v>
-      </c>
-      <c r="Y2">
-        <v>8.3492999999999998E-2</v>
-      </c>
-      <c r="Z2">
-        <v>0.10709399999999999</v>
-      </c>
-      <c r="AA2">
-        <v>2250</v>
-      </c>
-      <c r="AB2">
-        <v>650</v>
-      </c>
-      <c r="AC2">
-        <v>2000</v>
-      </c>
-      <c r="AD2">
-        <v>650</v>
-      </c>
-      <c r="AE2">
-        <v>2250</v>
-      </c>
-      <c r="AF2">
-        <v>160</v>
-      </c>
-      <c r="AG2">
-        <v>3300</v>
-      </c>
-      <c r="AH2">
-        <v>1500</v>
-      </c>
-      <c r="AI2">
-        <v>500</v>
-      </c>
-      <c r="AJ2">
-        <v>400</v>
-      </c>
-      <c r="AK2">
-        <v>900</v>
-      </c>
-      <c r="AL2">
-        <v>2250</v>
-      </c>
-      <c r="AM2">
-        <v>160</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>500</v>
-      </c>
-      <c r="AP2">
-        <v>4000</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
-        <v>7560</v>
-      </c>
-      <c r="AV2">
-        <v>4010</v>
-      </c>
-      <c r="AW2">
-        <v>2.4</v>
-      </c>
-      <c r="AX2">
-        <v>2.4</v>
-      </c>
-      <c r="AY2">
-        <v>2.4</v>
-      </c>
-      <c r="AZ2">
-        <v>2</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB2">
-        <v>108</v>
-      </c>
-      <c r="BC2">
-        <v>85</v>
-      </c>
-      <c r="BD2">
-        <v>-30</v>
-      </c>
-      <c r="BE2">
-        <v>1.5974999999999999</v>
-      </c>
-      <c r="BF2">
-        <v>1.4830000000000001</v>
-      </c>
-      <c r="BG2">
-        <v>0.1145</v>
-      </c>
-      <c r="BH2">
-        <v>-3.8</v>
-      </c>
-      <c r="BI2">
-        <v>0.30914999999999998</v>
-      </c>
-      <c r="BJ2">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="BK2">
-        <v>0</v>
-      </c>
-      <c r="BL2">
-        <v>6.0499999999999998E-2</v>
-      </c>
-      <c r="BM2">
-        <v>0.1285</v>
-      </c>
-      <c r="BN2">
-        <v>0.254</v>
-      </c>
-      <c r="BO2">
-        <v>0.33334999999999998</v>
-      </c>
-      <c r="BP2">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="BQ2">
-        <v>2.7</v>
-      </c>
-      <c r="BR2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="BS2">
-        <v>0.15</v>
-      </c>
-      <c r="BT2">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="BU2">
-        <v>133.69999999999999</v>
-      </c>
-      <c r="BV2">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="BW2">
-        <v>136.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>111</v>
-      </c>
-      <c r="U3" t="s">
-        <v>103</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>112</v>
-      </c>
-      <c r="U4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA7" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2284,16 +1771,931 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG6"/>
+  <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView topLeftCell="BR1" workbookViewId="0">
-      <selection activeCell="CB2" sqref="BT2:CB2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AZ7" sqref="AZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.5</v>
+      </c>
+      <c r="B2">
+        <v>85.95</v>
+      </c>
+      <c r="C2">
+        <v>144</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>19.2</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>12.5</v>
+      </c>
+      <c r="H2">
+        <v>12.5</v>
+      </c>
+      <c r="I2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K2">
+        <v>207</v>
+      </c>
+      <c r="L2">
+        <v>26.6</v>
+      </c>
+      <c r="M2">
+        <v>79.7</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>2000</v>
+      </c>
+      <c r="S2">
+        <v>650</v>
+      </c>
+      <c r="T2">
+        <v>3300</v>
+      </c>
+      <c r="U2">
+        <v>1300</v>
+      </c>
+      <c r="V2">
+        <v>300</v>
+      </c>
+      <c r="W2">
+        <v>300</v>
+      </c>
+      <c r="X2">
+        <v>650</v>
+      </c>
+      <c r="Y2">
+        <v>1600</v>
+      </c>
+      <c r="Z2">
+        <v>250</v>
+      </c>
+      <c r="AA2">
+        <v>4000</v>
+      </c>
+      <c r="AB2">
+        <v>500</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>6200</v>
+      </c>
+      <c r="AI2">
+        <v>3200</v>
+      </c>
+      <c r="AJ2">
+        <v>2.42</v>
+      </c>
+      <c r="AK2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AL2">
+        <v>2.33</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
+      <c r="AN2">
+        <v>70</v>
+      </c>
+      <c r="AO2">
+        <v>90.7</v>
+      </c>
+      <c r="AP2">
+        <v>-30</v>
+      </c>
+      <c r="AQ2">
+        <v>1.5861000000000001</v>
+      </c>
+      <c r="AR2">
+        <v>1.4876</v>
+      </c>
+      <c r="AS2">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="AT2">
+        <v>6.2</v>
+      </c>
+      <c r="AU2">
+        <v>0.32012499999999999</v>
+      </c>
+      <c r="AV2">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>6.8900000000000003E-2</v>
+      </c>
+      <c r="AY2">
+        <v>0.1464</v>
+      </c>
+      <c r="AZ2">
+        <v>0.22</v>
+      </c>
+      <c r="BA2">
+        <v>0.33450000000000002</v>
+      </c>
+      <c r="BB2">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="BC2">
+        <v>3.25</v>
+      </c>
+      <c r="BD2">
+        <v>3.04</v>
+      </c>
+      <c r="BE2">
+        <v>0.4</v>
+      </c>
+      <c r="BF2">
+        <v>63.87</v>
+      </c>
+      <c r="BG2">
+        <v>126.9</v>
+      </c>
+      <c r="BH2">
+        <v>63.87</v>
+      </c>
+      <c r="BI2">
+        <v>129.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BW7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BV6" sqref="BV6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2">
+        <v>5.7</v>
+      </c>
+      <c r="C2">
+        <v>86.25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>144</v>
+      </c>
+      <c r="G2">
+        <v>10.6</v>
+      </c>
+      <c r="H2">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="I2">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>0.10709399999999999</v>
+      </c>
+      <c r="K2">
+        <v>409.23145099999999</v>
+      </c>
+      <c r="L2">
+        <v>0.49662899999999999</v>
+      </c>
+      <c r="M2">
+        <v>8.5</v>
+      </c>
+      <c r="N2">
+        <v>8.5</v>
+      </c>
+      <c r="O2">
+        <v>18.5</v>
+      </c>
+      <c r="P2">
+        <v>18.5</v>
+      </c>
+      <c r="Q2">
+        <v>403</v>
+      </c>
+      <c r="R2">
+        <v>2.1347749999999999</v>
+      </c>
+      <c r="S2">
+        <v>276.91503</v>
+      </c>
+      <c r="T2">
+        <v>10.417676999999999</v>
+      </c>
+      <c r="U2" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2">
+        <v>24.8</v>
+      </c>
+      <c r="W2">
+        <v>68.8</v>
+      </c>
+      <c r="X2">
+        <v>3.0096000000000001E-2</v>
+      </c>
+      <c r="Y2">
+        <v>8.3492999999999998E-2</v>
+      </c>
+      <c r="Z2">
+        <v>0.10709399999999999</v>
+      </c>
+      <c r="AA2">
+        <v>2250</v>
+      </c>
+      <c r="AB2">
+        <v>650</v>
+      </c>
+      <c r="AC2">
+        <v>2000</v>
+      </c>
+      <c r="AD2">
+        <v>650</v>
+      </c>
+      <c r="AE2">
+        <v>2250</v>
+      </c>
+      <c r="AF2">
+        <v>160</v>
+      </c>
+      <c r="AG2">
+        <v>3300</v>
+      </c>
+      <c r="AH2">
+        <v>1500</v>
+      </c>
+      <c r="AI2">
+        <v>500</v>
+      </c>
+      <c r="AJ2">
+        <v>400</v>
+      </c>
+      <c r="AK2">
+        <v>900</v>
+      </c>
+      <c r="AL2">
+        <v>2250</v>
+      </c>
+      <c r="AM2">
+        <v>160</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>500</v>
+      </c>
+      <c r="AP2">
+        <v>4000</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>7560</v>
+      </c>
+      <c r="AV2">
+        <v>4010</v>
+      </c>
+      <c r="AW2">
+        <v>2.4</v>
+      </c>
+      <c r="AX2">
+        <v>2.4</v>
+      </c>
+      <c r="AY2">
+        <v>2.4</v>
+      </c>
+      <c r="AZ2">
+        <v>2</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BB2">
+        <v>108</v>
+      </c>
+      <c r="BC2">
+        <v>85</v>
+      </c>
+      <c r="BD2">
+        <v>-30</v>
+      </c>
+      <c r="BE2">
+        <v>1.5974999999999999</v>
+      </c>
+      <c r="BF2">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="BG2">
+        <v>0.1145</v>
+      </c>
+      <c r="BH2">
+        <v>-3.8</v>
+      </c>
+      <c r="BI2">
+        <v>0.30914999999999998</v>
+      </c>
+      <c r="BJ2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="BM2">
+        <v>0.1285</v>
+      </c>
+      <c r="BN2">
+        <v>0.254</v>
+      </c>
+      <c r="BO2">
+        <v>0.33334999999999998</v>
+      </c>
+      <c r="BP2">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="BQ2">
+        <v>2.7</v>
+      </c>
+      <c r="BR2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BS2">
+        <v>0.15</v>
+      </c>
+      <c r="BT2">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="BU2">
+        <v>133.69999999999999</v>
+      </c>
+      <c r="BV2">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="BW2">
+        <v>136.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="U3" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="U4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BA7" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CG6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BN2" sqref="A1:BN2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
@@ -2903,12 +3305,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="BV11" sqref="BV11"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:BN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify the SPS volume formula
</commit_message>
<xml_diff>
--- a/lc_margin/main/tests/files/LCmargin_train.xlsx
+++ b/lc_margin/main/tests/files/LCmargin_train.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="270" windowWidth="15780" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="4080" yWindow="270" windowWidth="15780" windowHeight="9030"/>
   </bookViews>
   <sheets>
-    <sheet name="upload" sheetId="4" r:id="rId1"/>
+    <sheet name="upload_T2" sheetId="4" r:id="rId1"/>
     <sheet name="upload_T1" sheetId="5" r:id="rId2"/>
     <sheet name="原始輸入表格" sheetId="2" r:id="rId3"/>
     <sheet name="轉換後表格_T2" sheetId="1" r:id="rId4"/>
@@ -1375,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1775,7 +1775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+    <sheetView topLeftCell="AU1" workbookViewId="0">
       <selection activeCell="AZ7" sqref="AZ7"/>
     </sheetView>
   </sheetViews>
@@ -2689,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BN2" sqref="A1:BN2"/>
+    <sheetView topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="BV2" sqref="BV2:BW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3309,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH6"/>
   <sheetViews>
-    <sheetView topLeftCell="BJ1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S2" sqref="S2:BN2"/>
     </sheetView>
   </sheetViews>

</xml_diff>